<commit_message>
added the update mode for updating vc numbers
</commit_message>
<xml_diff>
--- a/BCS_Approved_New_Hires.xlsx
+++ b/BCS_Approved_New_Hires.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C24" sqref="C24:C25"/>
@@ -928,6 +928,30 @@
         </is>
       </c>
     </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>1006914830</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Za Construction, LLC</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>67902</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Koren Development Company</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated for Pep8 compliance
</commit_message>
<xml_diff>
--- a/BCS_Approved_New_Hires.xlsx
+++ b/BCS_Approved_New_Hires.xlsx
@@ -412,10 +412,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B44"/>
+  <dimension ref="A1:B49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24:C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -952,6 +952,66 @@
         </is>
       </c>
     </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>1006460923</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>J.C. Driskill, Inc.</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>8796</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Tool-Smith</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>1006731870</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>First Response Rail Service</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>1006932041</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>C&amp;H Asphalt LLC</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>104543</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Consolidated Metal Services Inc</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>